<commit_message>
Graph and READM added
</commit_message>
<xml_diff>
--- a/Building Data/FDC_1min_21AUG2023.xlsx
+++ b/Building Data/FDC_1min_21AUG2023.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lore3652\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ustugrid\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C1CE3F-7419-4265-A920-BF13AA2DF48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439DC2A8-28A6-4FF7-B54F-4C3614F5D2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
+    <sheet name="README" sheetId="6" r:id="rId1"/>
     <sheet name="FDC_1Min_2023821" sheetId="1" r:id="rId2"/>
     <sheet name="August Power Output" sheetId="2" r:id="rId3"/>
     <sheet name="Line to Line Voltage" sheetId="3" r:id="rId4"/>
@@ -4383,7 +4383,7 @@
     <t>This project was made possible in whole or in part by a grant from the Minnesota Department of Commerce through the Minnesota Renewable Development Account, which is financed by Xcel Energy ratepayers. CMR sincerely thanks the Minnesota Department of Commerce, the Minnesota State Legislature, and Xcel Energy for their invaluable support in establishing the Center for Microgrid Research. Their contributions have been instrumental in advancing microgrid research and this data collection.</t>
   </si>
   <si>
-    <t>Data Title: FDC One Minute Data 21AUG2023</t>
+    <t>Data Title: FDC_1min_21AUG2023</t>
   </si>
 </sst>
 </file>
@@ -5447,16 +5447,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8956E034-9C9C-483B-8A7A-6E45F6EC3C6B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6158AA4A-6DC2-41B6-91A5-A36D6656013B}">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66" customWidth="1"/>
+    <col min="1" max="1" width="65" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -5484,7 +5484,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1451</v>
       </c>

</xml_diff>